<commit_message>
rm useless english descr a86cdf2c8ce16f2800f2bd25f9a0e4627487a13f
</commit_message>
<xml_diff>
--- a/nr-update-profiles/ig/StructureDefinition-fr-medication-reconciliation-statement.xlsx
+++ b/nr-update-profiles/ig/StructureDefinition-fr-medication-reconciliation-statement.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2823" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="533">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-05T13:40:24+00:00</t>
+    <t>2025-02-05T13:46:54+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -887,9 +887,6 @@
     <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
   </si>
   <si>
-    <t>référence la ressource Patient selon la profile fr-patient défini par Interop'Santé</t>
-  </si>
-  <si>
     <t>Reference.reference</t>
   </si>
   <si>
@@ -937,9 +934,6 @@
 Reference is intended to point to a structure that can potentially be expressed as a FHIR resource, though there is no need for it to exist as an actual FHIR resource instance - except in as much as an application wishes to actual find the target of the reference. The content referred to be the identifier must meet the logical constraints implied by any limitations on what resource types are permitted for the reference.  For example, it would not be legitimate to send the identifier for a drug prescription if the type were Reference(Observation|DiagnosticReport).  One of the use-cases for Reference.identifier is the situation where no FHIR representation exists (where the type is Reference (Any).</t>
   </si>
   <si>
-    <t>Identification du patient exclusivement par référence à une ressource Patient selon le profil fr-patient défini par Interop'Santé</t>
-  </si>
-  <si>
     <t>Reference.identifier</t>
   </si>
   <si>
@@ -1575,10 +1569,10 @@
 Quantity {https://hl7.fr/fhir/fr/medication/StructureDefinition/FrSimpleQuantityUcum}</t>
   </si>
   <si>
-    <t>Precise amount of medication per dose</t>
-  </si>
-  <si>
-    <t>Amount of medication per dose. No use of element 'comparator' in the simpleQuantity definitions.</t>
+    <t>Amount of medication per dose</t>
+  </si>
+  <si>
+    <t>Amount of medication per dose.</t>
   </si>
   <si>
     <t>Note that this specifies the quantity of the specified medication, not the quantity for each active ingredient(s). Each ingredient amount can be communicated in the Medication resource. For example, if one wants to communicate that a tablet was 375 mg, where the dose was one tablet, you can use the Medication resource to document that the tablet was comprised of 375 mg of drug XYZ. Alternatively if the dose was 375 mg, then you may only need to use the Medication resource to indicate this was a tablet. If the example were an IV such as dopamine and you wanted to communicate that 400mg of dopamine was mixed in 500 ml of some IV solution, then this would all be communicated in the Medication resource. If the administration is not intended to be instantaneous (rate is present or timing has a duration), this can be specified to convey the total amount to be administered over the period of time as indicated by the schedule e.g. 500 ml in dose, with timing used to convey that this should be done over 4 hours.</t>
@@ -1600,10 +1594,10 @@
 Range {https://hl7.fr/fhir/fr/medication/StructureDefinition/FrRangeUcum}Quantity {https://hl7.fr/fhir/fr/medication/StructureDefinition/FrSimpleQuantityUcum}</t>
   </si>
   <si>
-    <t>Precise amount of medication per unit of time</t>
-  </si>
-  <si>
-    <t>Amount of medication per unit of time No use of element 'comparator' in the simpleQuantity definitions.</t>
+    <t>Amount of medication per unit of time</t>
+  </si>
+  <si>
+    <t>Amount of medication per unit of time.</t>
   </si>
   <si>
     <t>It is possible to supply both a rate and a doseQuantity to provide full details about how the medication is to be administered and supplied. If the rate is intended to change over time, depending on local rules/regulations, each change should be captured as a new version of the MedicationRequest with an updated rate, or captured with a new MedicationRequest with the new rate.@@ -5407,9 +5401,7 @@
       <c r="N30" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="O30" t="s" s="2">
-        <v>276</v>
-      </c>
+      <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>19</v>
       </c>
@@ -5457,7 +5449,7 @@
         <v>19</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>76</v>
@@ -5466,7 +5458,7 @@
         <v>86</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>98</v>
@@ -5486,10 +5478,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5515,13 +5507,13 @@
         <v>128</v>
       </c>
       <c r="L31" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="M31" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5532,7 +5524,7 @@
         <v>19</v>
       </c>
       <c r="S31" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="T31" t="s" s="2">
         <v>19</v>
@@ -5550,28 +5542,28 @@
         <v>144</v>
       </c>
       <c r="Y31" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Z31" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="Z31" t="s" s="2">
+      <c r="AA31" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE31" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF31" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>76</v>
@@ -5600,10 +5592,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5629,17 +5621,15 @@
         <v>204</v>
       </c>
       <c r="L32" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M32" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="M32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="N32" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="O32" t="s" s="2">
-        <v>291</v>
-      </c>
+      <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>19</v>
       </c>
@@ -5687,7 +5677,7 @@
         <v>19</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>76</v>
@@ -5705,7 +5695,7 @@
         <v>19</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>19</v>
@@ -5716,10 +5706,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5745,13 +5735,13 @@
         <v>100</v>
       </c>
       <c r="L33" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="N33" t="s" s="2">
         <v>295</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5801,7 +5791,7 @@
         <v>19</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>76</v>
@@ -5830,10 +5820,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5856,13 +5846,13 @@
         <v>87</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>302</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5913,7 +5903,7 @@
         <v>19</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>76</v>
@@ -5928,10 +5918,10 @@
         <v>98</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>19</v>
@@ -5942,10 +5932,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5968,16 +5958,16 @@
         <v>87</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>307</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -6027,7 +6017,7 @@
         <v>19</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>76</v>
@@ -6042,13 +6032,13 @@
         <v>98</v>
       </c>
       <c r="AK35" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>19</v>
@@ -6056,10 +6046,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6082,13 +6072,13 @@
         <v>87</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M36" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6139,7 +6129,7 @@
         <v>19</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>76</v>
@@ -6157,10 +6147,10 @@
         <v>19</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>19</v>
@@ -6168,10 +6158,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6194,19 +6184,19 @@
         <v>19</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="O37" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>324</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>19</v>
@@ -6255,7 +6245,7 @@
         <v>19</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>76</v>
@@ -6273,10 +6263,10 @@
         <v>19</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>19</v>
@@ -6284,10 +6274,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6298,7 +6288,7 @@
         <v>86</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>87</v>
@@ -6310,19 +6300,19 @@
         <v>19</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="O38" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>19</v>
@@ -6362,7 +6352,7 @@
         <v>19</v>
       </c>
       <c r="AC38" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AD38" t="s" s="2">
         <v>19</v>
@@ -6371,7 +6361,7 @@
         <v>113</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>76</v>
@@ -6389,7 +6379,7 @@
         <v>19</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>19</v>
@@ -6400,13 +6390,13 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D39" t="s" s="2">
         <v>19</v>
@@ -6428,19 +6418,19 @@
         <v>19</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="O39" t="s" s="2">
         <v>340</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>19</v>
@@ -6489,7 +6479,7 @@
         <v>19</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>76</v>
@@ -6507,7 +6497,7 @@
         <v>19</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>19</v>
@@ -6518,10 +6508,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6630,10 +6620,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6744,10 +6734,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6829,7 +6819,7 @@
         <v>19</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>76</v>
@@ -6838,7 +6828,7 @@
         <v>86</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>98</v>
@@ -6858,10 +6848,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6887,13 +6877,13 @@
         <v>128</v>
       </c>
       <c r="L43" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6922,28 +6912,28 @@
         <v>144</v>
       </c>
       <c r="Y43" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Z43" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="Z43" t="s" s="2">
+      <c r="AA43" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF43" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>76</v>
@@ -6972,10 +6962,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7001,16 +6991,16 @@
         <v>204</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="N44" t="s" s="2">
-        <v>290</v>
-      </c>
       <c r="O44" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>19</v>
@@ -7059,7 +7049,7 @@
         <v>19</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>76</v>
@@ -7077,7 +7067,7 @@
         <v>19</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>19</v>
@@ -7088,10 +7078,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7117,13 +7107,13 @@
         <v>100</v>
       </c>
       <c r="L45" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="N45" t="s" s="2">
         <v>295</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7173,7 +7163,7 @@
         <v>19</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>76</v>
@@ -7202,13 +7192,13 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D46" t="s" s="2">
         <v>19</v>
@@ -7230,19 +7220,19 @@
         <v>19</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="M46" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="N46" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="M46" t="s" s="2">
+      <c r="O46" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="O46" t="s" s="2">
-        <v>362</v>
       </c>
       <c r="P46" t="s" s="2">
         <v>19</v>
@@ -7291,7 +7281,7 @@
         <v>19</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>76</v>
@@ -7309,7 +7299,7 @@
         <v>19</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>19</v>
@@ -7320,10 +7310,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7432,10 +7422,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7546,10 +7536,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7631,7 +7621,7 @@
         <v>19</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>76</v>
@@ -7640,7 +7630,7 @@
         <v>86</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>98</v>
@@ -7660,10 +7650,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7689,13 +7679,13 @@
         <v>128</v>
       </c>
       <c r="L50" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="M50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7724,28 +7714,28 @@
         <v>144</v>
       </c>
       <c r="Y50" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Z50" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="Z50" t="s" s="2">
+      <c r="AA50" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF50" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>76</v>
@@ -7774,10 +7764,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7803,16 +7793,16 @@
         <v>204</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="M51" t="s" s="2">
+      <c r="N51" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="N51" t="s" s="2">
-        <v>290</v>
-      </c>
       <c r="O51" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>19</v>
@@ -7861,7 +7851,7 @@
         <v>19</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>76</v>
@@ -7879,7 +7869,7 @@
         <v>19</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>19</v>
@@ -7890,10 +7880,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7919,13 +7909,13 @@
         <v>100</v>
       </c>
       <c r="L52" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="N52" t="s" s="2">
         <v>295</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7975,7 +7965,7 @@
         <v>19</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>76</v>
@@ -8004,10 +7994,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8033,13 +8023,13 @@
         <v>236</v>
       </c>
       <c r="L53" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="N53" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -8068,10 +8058,10 @@
         <v>152</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="Z53" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>19</v>
@@ -8089,7 +8079,7 @@
         <v>19</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>76</v>
@@ -8104,13 +8094,13 @@
         <v>98</v>
       </c>
       <c r="AK53" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="AM53" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>19</v>
@@ -8118,10 +8108,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8144,16 +8134,16 @@
         <v>19</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="M54" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="L54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8203,7 +8193,7 @@
         <v>19</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>76</v>
@@ -8218,13 +8208,13 @@
         <v>98</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>19</v>
@@ -8232,10 +8222,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8258,19 +8248,19 @@
         <v>19</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="M55" t="s" s="2">
+      <c r="O55" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>19</v>
@@ -8319,7 +8309,7 @@
         <v>19</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>76</v>
@@ -8334,10 +8324,10 @@
         <v>98</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>19</v>
@@ -8348,10 +8338,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8374,16 +8364,16 @@
         <v>19</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -8433,7 +8423,7 @@
         <v>19</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>76</v>
@@ -8451,7 +8441,7 @@
         <v>19</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>19</v>
@@ -8462,10 +8452,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8574,10 +8564,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8688,14 +8678,14 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
@@ -8717,10 +8707,10 @@
         <v>107</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="N59" t="s" s="2">
         <v>110</v>
@@ -8775,7 +8765,7 @@
         <v>19</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>76</v>
@@ -8804,10 +8794,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8830,17 +8820,17 @@
         <v>87</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="M60" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>19</v>
@@ -8889,7 +8879,7 @@
         <v>19</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>76</v>
@@ -8907,21 +8897,21 @@
         <v>19</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8947,14 +8937,14 @@
         <v>100</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P61" t="s" s="2">
         <v>19</v>
@@ -9003,7 +8993,7 @@
         <v>19</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>76</v>
@@ -9021,21 +9011,21 @@
         <v>19</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9061,16 +9051,16 @@
         <v>236</v>
       </c>
       <c r="L62" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="N62" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="O62" t="s" s="2">
         <v>423</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="O62" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>19</v>
@@ -9098,28 +9088,28 @@
         <v>152</v>
       </c>
       <c r="Y62" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF62" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF62" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>76</v>
@@ -9137,21 +9127,21 @@
         <v>19</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9177,10 +9167,10 @@
         <v>100</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9231,7 +9221,7 @@
         <v>19</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>76</v>
@@ -9249,21 +9239,21 @@
         <v>19</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9286,19 +9276,19 @@
         <v>87</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="L64" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="N64" t="s" s="2">
         <v>436</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="O64" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="O64" t="s" s="2">
-        <v>439</v>
       </c>
       <c r="P64" t="s" s="2">
         <v>19</v>
@@ -9347,7 +9337,7 @@
         <v>19</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>76</v>
@@ -9365,7 +9355,7 @@
         <v>19</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>19</v>
@@ -9376,10 +9366,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9402,16 +9392,16 @@
         <v>87</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="M65" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="L65" t="s" s="2">
+      <c r="N65" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>445</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9440,28 +9430,28 @@
         <v>152</v>
       </c>
       <c r="Y65" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF65" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="Z65" t="s" s="2">
-        <v>447</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF65" t="s" s="2">
-        <v>448</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>76</v>
@@ -9479,21 +9469,21 @@
         <v>19</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9519,16 +9509,16 @@
         <v>236</v>
       </c>
       <c r="L66" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="N66" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="M66" t="s" s="2">
+      <c r="O66" t="s" s="2">
         <v>453</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>454</v>
-      </c>
-      <c r="O66" t="s" s="2">
-        <v>455</v>
       </c>
       <c r="P66" t="s" s="2">
         <v>19</v>
@@ -9556,28 +9546,28 @@
         <v>152</v>
       </c>
       <c r="Y66" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF66" t="s" s="2">
         <v>456</v>
-      </c>
-      <c r="Z66" t="s" s="2">
-        <v>457</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF66" t="s" s="2">
-        <v>458</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>76</v>
@@ -9595,21 +9585,21 @@
         <v>19</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9635,14 +9625,14 @@
         <v>236</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P67" t="s" s="2">
         <v>19</v>
@@ -9670,28 +9660,28 @@
         <v>152</v>
       </c>
       <c r="Y67" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF67" t="s" s="2">
         <v>465</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>467</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>76</v>
@@ -9709,21 +9699,21 @@
         <v>19</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -9749,16 +9739,16 @@
         <v>236</v>
       </c>
       <c r="L68" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="N68" t="s" s="2">
         <v>471</v>
       </c>
-      <c r="M68" t="s" s="2">
+      <c r="O68" t="s" s="2">
         <v>472</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>473</v>
-      </c>
-      <c r="O68" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="P68" t="s" s="2">
         <v>19</v>
@@ -9786,28 +9776,28 @@
         <v>152</v>
       </c>
       <c r="Y68" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF68" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>476</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>76</v>
@@ -9825,21 +9815,21 @@
         <v>19</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -9862,13 +9852,13 @@
         <v>87</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="M69" t="s" s="2">
         <v>481</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>482</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>483</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -9919,7 +9909,7 @@
         <v>19</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>76</v>
@@ -9943,15 +9933,15 @@
         <v>19</v>
       </c>
       <c r="AN69" t="s" s="2">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10060,10 +10050,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10174,10 +10164,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10203,14 +10193,14 @@
         <v>236</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="P72" t="s" s="2">
         <v>19</v>
@@ -10238,28 +10228,28 @@
         <v>152</v>
       </c>
       <c r="Y72" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="Z72" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AA72" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE72" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF72" t="s" s="2">
         <v>492</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>494</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>76</v>
@@ -10283,15 +10273,15 @@
         <v>19</v>
       </c>
       <c r="AN72" t="s" s="2">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10314,19 +10304,19 @@
         <v>87</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="L73" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>497</v>
       </c>
-      <c r="L73" t="s" s="2">
+      <c r="N73" t="s" s="2">
         <v>498</v>
       </c>
-      <c r="M73" t="s" s="2">
+      <c r="O73" t="s" s="2">
         <v>499</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="O73" t="s" s="2">
-        <v>501</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>19</v>
@@ -10375,7 +10365,7 @@
         <v>19</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>76</v>
@@ -10393,21 +10383,21 @@
         <v>19</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN73" t="s" s="2">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10430,19 +10420,19 @@
         <v>87</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="L74" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="M74" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="L74" t="s" s="2">
+      <c r="N74" t="s" s="2">
         <v>506</v>
       </c>
-      <c r="M74" t="s" s="2">
+      <c r="O74" t="s" s="2">
         <v>507</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>508</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>509</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>19</v>
@@ -10491,7 +10481,7 @@
         <v>19</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>76</v>
@@ -10509,21 +10499,21 @@
         <v>19</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN74" t="s" s="2">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10546,19 +10536,19 @@
         <v>87</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>512</v>
+      </c>
+      <c r="L75" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="M75" t="s" s="2">
         <v>514</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="N75" t="s" s="2">
         <v>515</v>
       </c>
-      <c r="M75" t="s" s="2">
+      <c r="O75" t="s" s="2">
         <v>516</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>518</v>
       </c>
       <c r="P75" t="s" s="2">
         <v>19</v>
@@ -10607,7 +10597,7 @@
         <v>19</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>76</v>
@@ -10625,21 +10615,21 @@
         <v>19</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AM75" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10662,19 +10652,19 @@
         <v>87</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="L76" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="M76" t="s" s="2">
         <v>523</v>
       </c>
-      <c r="L76" t="s" s="2">
+      <c r="N76" t="s" s="2">
         <v>524</v>
       </c>
-      <c r="M76" t="s" s="2">
+      <c r="O76" t="s" s="2">
         <v>525</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>526</v>
-      </c>
-      <c r="O76" t="s" s="2">
-        <v>527</v>
       </c>
       <c r="P76" t="s" s="2">
         <v>19</v>
@@ -10723,7 +10713,7 @@
         <v>19</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>76</v>
@@ -10741,7 +10731,7 @@
         <v>19</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>19</v>
@@ -10752,10 +10742,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10778,17 +10768,17 @@
         <v>87</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="P77" t="s" s="2">
         <v>19</v>
@@ -10837,7 +10827,7 @@
         <v>19</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>76</v>
@@ -10855,7 +10845,7 @@
         <v>19</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>19</v>

</xml_diff>